<commit_message>
Scrape of Dog Image
</commit_message>
<xml_diff>
--- a/Research Progress/Gantt Chart.xlsx
+++ b/Research Progress/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Multipet-Feeder\Research Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98E2ACA-CE94-4A3E-B630-5FC722C8D19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65903D9-2958-4B70-9E0A-92AAF638C043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{52E49B7B-73AD-4BD1-9DED-2BD0572E1B28}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{52E49B7B-73AD-4BD1-9DED-2BD0572E1B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
-    <t>Project Selection and Drafting of Proposal</t>
-  </si>
-  <si>
     <t>Choosing the project idea.</t>
   </si>
   <si>
@@ -50,36 +47,21 @@
     <t>Supervisor Meeting for Proposal Approval</t>
   </si>
   <si>
-    <t>Presenting the proposal to the supervisor and getting approval.</t>
-  </si>
-  <si>
     <t>Project Kick-Off and Initial Planning</t>
   </si>
   <si>
-    <t>Finalizing the project scope and objectives post-approval.</t>
-  </si>
-  <si>
     <t>Outlining the detailed plan and schedule for the project.</t>
   </si>
   <si>
     <t>Research on Machine Vision Algorithms</t>
   </si>
   <si>
-    <t>Initiating research on machine vision for species recognition.</t>
-  </si>
-  <si>
     <t>Supervisor meeting to discuss research direction and findings.</t>
   </si>
   <si>
-    <t>Starting Development of Health Assessment Algorithms</t>
-  </si>
-  <si>
     <t>Beginning research and development on health assessment algorithms.</t>
   </si>
   <si>
-    <t>Health-Optimized Nutritional Dispensing Research</t>
-  </si>
-  <si>
     <t>Supervisor meeting to discuss nutritional requirements and algorithm design.</t>
   </si>
   <si>
@@ -101,15 +83,9 @@
     <t>Improving machine vision and health assessment algorithms.</t>
   </si>
   <si>
-    <t>System Integration</t>
-  </si>
-  <si>
     <t>Beginning the integration of different components (vision system, health assessment, and feeder).</t>
   </si>
   <si>
-    <t>Preparing for System Testing</t>
-  </si>
-  <si>
     <t>Setting up testing environments and protocols.</t>
   </si>
   <si>
@@ -122,21 +98,12 @@
     <t>Supervisor meeting to discuss initial testing results.</t>
   </si>
   <si>
-    <t>Final Adjustments and Completion</t>
-  </si>
-  <si>
-    <t>Finalizing the system and preparing for project presentation.</t>
-  </si>
-  <si>
     <t>Supervisor meeting for final review and approval.</t>
   </si>
   <si>
     <t>Documentation and Presentation Preparation</t>
   </si>
   <si>
-    <t>Compiling project documentation and preparing for the final presentation.</t>
-  </si>
-  <si>
     <t>TASKS</t>
   </si>
   <si>
@@ -225,13 +192,189 @@
   </si>
   <si>
     <t>KEYS</t>
+  </si>
+  <si>
+    <r>
+      <t>Finalizing the project scope and objectives post-approval</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-D2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Presenting the proposal to the supervisor and getting approval.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -M1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Project Selection and Drafting of Proposald-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>System Integration-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Finalizing the system and preparing for project presentation.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-M4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Initiating research on machine vision for species recognition</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- D3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Health-Optimized Nutritional Dispensing Research-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Starting Development of Health Assessment Algorithms-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Preparing for System Testing</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-D9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Final Adjustments and Completion-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Compiling project documentation and preparing for the final presentation.-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D10</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +431,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +460,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,7 +525,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -388,11 +545,13 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -712,10 +871,10 @@
   <dimension ref="A1:BR51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L46" sqref="L46"/>
+      <selection pane="bottomRight" activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -730,89 +889,89 @@
   <sheetData>
     <row r="1" spans="1:70" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
@@ -858,7 +1017,7 @@
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -867,7 +1026,7 @@
     </row>
     <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="6">
         <v>45209</v>
@@ -884,7 +1043,7 @@
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6">
         <v>45214</v>
@@ -907,7 +1066,7 @@
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="6">
         <v>45220</v>
@@ -923,8 +1082,8 @@
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
+      <c r="A7" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="B7" s="6">
         <v>45221</v>
@@ -947,7 +1106,7 @@
     </row>
     <row r="9" spans="1:70" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -956,7 +1115,7 @@
     </row>
     <row r="10" spans="1:70" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B10" s="6">
         <v>45221</v>
@@ -973,7 +1132,7 @@
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11" s="6">
         <v>45229</v>
@@ -996,7 +1155,7 @@
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B13" s="6">
         <v>45229</v>
@@ -1007,7 +1166,7 @@
     </row>
     <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B14" s="6">
         <v>45229</v>
@@ -1026,7 +1185,7 @@
     </row>
     <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B15" s="6">
         <v>45257</v>
@@ -1049,7 +1208,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B17" s="6">
         <v>45257</v>
@@ -1060,7 +1219,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B18" s="6">
         <v>45257</v>
@@ -1086,7 +1245,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="B20" s="6">
         <v>45285</v>
@@ -1097,7 +1256,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B21" s="6">
         <v>45285</v>
@@ -1114,7 +1273,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B22" s="6">
         <v>45285</v>
@@ -1137,7 +1296,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B24" s="6">
         <v>45299</v>
@@ -1148,7 +1307,7 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B25" s="6">
         <v>45299</v>
@@ -1167,7 +1326,7 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B26" s="6">
         <v>45320</v>
@@ -1190,7 +1349,7 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B28" s="6">
         <v>45320</v>
@@ -1201,7 +1360,7 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B29" s="6">
         <v>45320</v>
@@ -1224,8 +1383,8 @@
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>21</v>
+      <c r="A31" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="B31" s="6">
         <v>45334</v>
@@ -1236,7 +1395,7 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B32" s="6">
         <v>45334</v>
@@ -1261,7 +1420,7 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B34" s="6">
         <v>45355</v>
@@ -1274,7 +1433,7 @@
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B35" s="6">
         <v>45355</v>
@@ -1297,7 +1456,7 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B37" s="6">
         <v>45362</v>
@@ -1308,7 +1467,7 @@
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B38" s="6">
         <v>45362</v>
@@ -1325,7 +1484,7 @@
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B39" s="6">
         <v>45369</v>
@@ -1348,7 +1507,7 @@
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B41" s="6">
         <v>45376</v>
@@ -1358,8 +1517,8 @@
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>29</v>
+      <c r="A42" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="B42" s="6">
         <v>45376</v>
@@ -1376,7 +1535,7 @@
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B43" s="6">
         <v>45383</v>
@@ -1399,7 +1558,7 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B45" s="6">
         <v>45390</v>
@@ -1410,31 +1569,54 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B46" s="6">
-        <v>45390</v>
+        <v>45209</v>
       </c>
       <c r="C46" s="6">
         <v>45397</v>
       </c>
       <c r="D46" s="8">
         <f>+C46-B46</f>
-        <v>7</v>
+        <v>188</v>
       </c>
       <c r="E46" s="7"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="10"/>
+      <c r="V46" s="10"/>
+      <c r="W46" s="10"/>
+      <c r="X46" s="10"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="10"/>
+      <c r="AA46" s="10"/>
+      <c r="AB46" s="10"/>
       <c r="AC46" s="10"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" s="13"/>
+      <c r="A50" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="15"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="15" t="s">
-        <v>61</v>
+      <c r="A51" s="13"/>
+      <c r="B51" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>